<commit_message>
time and depth additional tests
</commit_message>
<xml_diff>
--- a/Week-4-Results/depth.xlsx
+++ b/Week-4-Results/depth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amyta\OneDrive - Georgia Institute of Technology\Documents\mc-chess\Week-4-Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/atang68_gatech_edu/Documents/Documents/mc-chess/Week-4-Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62D12335-A1FB-4344-8EA2-7F05DAD1FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{62D12335-A1FB-4344-8EA2-7F05DAD1FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D1AAEA1-0DD0-4009-A871-8E8910C68F5D}"/>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="984" windowWidth="23112" windowHeight="11256"/>
+    <workbookView xWindow="0" yWindow="1152" windowWidth="23040" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="depth" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,10 +680,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>depth!$B$2:$B$204</c:f>
+              <c:f>depth!$B$2:$B$306</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="203"/>
+                <c:ptCount val="305"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
                 </c:pt>
@@ -1283,6 +1283,306 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>757</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>475</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>489</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>481</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>463</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>485</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>479</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3899</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>3958</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>3886</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>3933</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3874</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>3896</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3937</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>3938</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>3947</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>3939</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>3940</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>3907</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>3815</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>3951</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>3867</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>3886</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>3916</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>3948</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>3820</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>3966</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>4016</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>3788</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>3914</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3926</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>3938</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>3864</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>3964</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>3842</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>3986</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>3904</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>3846</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>3953</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>3813</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>3945</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>3925</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>3911</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>3857</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>3946</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>3853</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>3816</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>3903</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>3865</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>3961</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>3955</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>3905</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>3870</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>3826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,7 +1590,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-245B-4ACC-8A51-15F341ED6E9E}"/>
+              <c16:uniqueId val="{00000000-C401-448F-B0E1-9E977418FD22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1322,10 +1622,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>depth!$C$2:$C$204</c:f>
+              <c:f>depth!$C$2:$C$306</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="203"/>
+                <c:ptCount val="305"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1925,6 +2225,306 @@
                 </c:pt>
                 <c:pt idx="202">
                   <c:v>826</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>389</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>363</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>371</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>381</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>367</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>427</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>3934</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>3888</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>3807</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>3769</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>3897</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3914</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>3965</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>3900</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>3778</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>3935</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>3899</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>3867</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>3793</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>3893</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>3843</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>3913</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>3938</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>3895</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>3895</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>3809</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>3855</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>3904</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>3998</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>3781</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>3788</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>3857</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>3964</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>3878</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>3871</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>3879</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>4006</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>3958</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>3849</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>3978</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>3991</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>3799</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>3944</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>3761</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>3839</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>3824</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>3877</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>3863</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>3764</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>3812</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>3852</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>3858</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>3919</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>3933</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>3963</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1932,7 +2532,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-245B-4ACC-8A51-15F341ED6E9E}"/>
+              <c16:uniqueId val="{00000001-C401-448F-B0E1-9E977418FD22}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1945,11 +2545,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1564436575"/>
-        <c:axId val="2067762623"/>
+        <c:axId val="652427455"/>
+        <c:axId val="821367727"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1564436575"/>
+        <c:axId val="652427455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,7 +2591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2067762623"/>
+        <c:crossAx val="821367727"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1999,7 +2599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2067762623"/>
+        <c:axId val="821367727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2050,7 +2650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564436575"/>
+        <c:crossAx val="652427455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2697,23 +3297,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>148590</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FED0AB4-D9AF-E45A-8B33-53DA5884AA26}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B2CEA16-4E0C-1BFE-5045-B0C4AD1A076A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2732,6 +3332,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3030,11 +3634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I204"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8871,6 +9475,2906 @@
         <v>9</v>
       </c>
     </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>1</v>
+      </c>
+      <c r="B206">
+        <v>483</v>
+      </c>
+      <c r="C206">
+        <v>400</v>
+      </c>
+      <c r="D206">
+        <v>49117</v>
+      </c>
+      <c r="E206">
+        <v>50000</v>
+      </c>
+      <c r="F206">
+        <v>20</v>
+      </c>
+      <c r="G206">
+        <v>15</v>
+      </c>
+      <c r="H206">
+        <v>20</v>
+      </c>
+      <c r="I206" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>2</v>
+      </c>
+      <c r="B207">
+        <v>421</v>
+      </c>
+      <c r="C207">
+        <v>389</v>
+      </c>
+      <c r="D207">
+        <v>49190</v>
+      </c>
+      <c r="E207">
+        <v>50000</v>
+      </c>
+      <c r="F207">
+        <v>20</v>
+      </c>
+      <c r="G207">
+        <v>15</v>
+      </c>
+      <c r="H207">
+        <v>20</v>
+      </c>
+      <c r="I207" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>478</v>
+      </c>
+      <c r="C208">
+        <v>402</v>
+      </c>
+      <c r="D208">
+        <v>49120</v>
+      </c>
+      <c r="E208">
+        <v>50000</v>
+      </c>
+      <c r="F208">
+        <v>20</v>
+      </c>
+      <c r="G208">
+        <v>15</v>
+      </c>
+      <c r="H208">
+        <v>20</v>
+      </c>
+      <c r="I208" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>4</v>
+      </c>
+      <c r="B209">
+        <v>436</v>
+      </c>
+      <c r="C209">
+        <v>347</v>
+      </c>
+      <c r="D209">
+        <v>49217</v>
+      </c>
+      <c r="E209">
+        <v>50000</v>
+      </c>
+      <c r="F209">
+        <v>20</v>
+      </c>
+      <c r="G209">
+        <v>15</v>
+      </c>
+      <c r="H209">
+        <v>20</v>
+      </c>
+      <c r="I209" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>5</v>
+      </c>
+      <c r="B210">
+        <v>412</v>
+      </c>
+      <c r="C210">
+        <v>380</v>
+      </c>
+      <c r="D210">
+        <v>49208</v>
+      </c>
+      <c r="E210">
+        <v>50000</v>
+      </c>
+      <c r="F210">
+        <v>20</v>
+      </c>
+      <c r="G210">
+        <v>15</v>
+      </c>
+      <c r="H210">
+        <v>20</v>
+      </c>
+      <c r="I210" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>6</v>
+      </c>
+      <c r="B211">
+        <v>452</v>
+      </c>
+      <c r="C211">
+        <v>383</v>
+      </c>
+      <c r="D211">
+        <v>49165</v>
+      </c>
+      <c r="E211">
+        <v>50000</v>
+      </c>
+      <c r="F211">
+        <v>20</v>
+      </c>
+      <c r="G211">
+        <v>15</v>
+      </c>
+      <c r="H211">
+        <v>20</v>
+      </c>
+      <c r="I211" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>7</v>
+      </c>
+      <c r="B212">
+        <v>467</v>
+      </c>
+      <c r="C212">
+        <v>395</v>
+      </c>
+      <c r="D212">
+        <v>49138</v>
+      </c>
+      <c r="E212">
+        <v>50000</v>
+      </c>
+      <c r="F212">
+        <v>20</v>
+      </c>
+      <c r="G212">
+        <v>15</v>
+      </c>
+      <c r="H212">
+        <v>20</v>
+      </c>
+      <c r="I212" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>8</v>
+      </c>
+      <c r="B213">
+        <v>427</v>
+      </c>
+      <c r="C213">
+        <v>380</v>
+      </c>
+      <c r="D213">
+        <v>49193</v>
+      </c>
+      <c r="E213">
+        <v>50000</v>
+      </c>
+      <c r="F213">
+        <v>20</v>
+      </c>
+      <c r="G213">
+        <v>15</v>
+      </c>
+      <c r="H213">
+        <v>20</v>
+      </c>
+      <c r="I213" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>9</v>
+      </c>
+      <c r="B214">
+        <v>440</v>
+      </c>
+      <c r="C214">
+        <v>353</v>
+      </c>
+      <c r="D214">
+        <v>49207</v>
+      </c>
+      <c r="E214">
+        <v>50000</v>
+      </c>
+      <c r="F214">
+        <v>20</v>
+      </c>
+      <c r="G214">
+        <v>15</v>
+      </c>
+      <c r="H214">
+        <v>20</v>
+      </c>
+      <c r="I214" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>10</v>
+      </c>
+      <c r="B215">
+        <v>451</v>
+      </c>
+      <c r="C215">
+        <v>439</v>
+      </c>
+      <c r="D215">
+        <v>49110</v>
+      </c>
+      <c r="E215">
+        <v>50000</v>
+      </c>
+      <c r="F215">
+        <v>20</v>
+      </c>
+      <c r="G215">
+        <v>15</v>
+      </c>
+      <c r="H215">
+        <v>20</v>
+      </c>
+      <c r="I215" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>11</v>
+      </c>
+      <c r="B216">
+        <v>461</v>
+      </c>
+      <c r="C216">
+        <v>363</v>
+      </c>
+      <c r="D216">
+        <v>49176</v>
+      </c>
+      <c r="E216">
+        <v>50000</v>
+      </c>
+      <c r="F216">
+        <v>20</v>
+      </c>
+      <c r="G216">
+        <v>15</v>
+      </c>
+      <c r="H216">
+        <v>20</v>
+      </c>
+      <c r="I216" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>12</v>
+      </c>
+      <c r="B217">
+        <v>457</v>
+      </c>
+      <c r="C217">
+        <v>377</v>
+      </c>
+      <c r="D217">
+        <v>49166</v>
+      </c>
+      <c r="E217">
+        <v>50000</v>
+      </c>
+      <c r="F217">
+        <v>20</v>
+      </c>
+      <c r="G217">
+        <v>15</v>
+      </c>
+      <c r="H217">
+        <v>20</v>
+      </c>
+      <c r="I217" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>13</v>
+      </c>
+      <c r="B218">
+        <v>468</v>
+      </c>
+      <c r="C218">
+        <v>388</v>
+      </c>
+      <c r="D218">
+        <v>49144</v>
+      </c>
+      <c r="E218">
+        <v>50000</v>
+      </c>
+      <c r="F218">
+        <v>20</v>
+      </c>
+      <c r="G218">
+        <v>15</v>
+      </c>
+      <c r="H218">
+        <v>20</v>
+      </c>
+      <c r="I218" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>14</v>
+      </c>
+      <c r="B219">
+        <v>443</v>
+      </c>
+      <c r="C219">
+        <v>383</v>
+      </c>
+      <c r="D219">
+        <v>49174</v>
+      </c>
+      <c r="E219">
+        <v>50000</v>
+      </c>
+      <c r="F219">
+        <v>20</v>
+      </c>
+      <c r="G219">
+        <v>15</v>
+      </c>
+      <c r="H219">
+        <v>20</v>
+      </c>
+      <c r="I219" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>15</v>
+      </c>
+      <c r="B220">
+        <v>445</v>
+      </c>
+      <c r="C220">
+        <v>388</v>
+      </c>
+      <c r="D220">
+        <v>49167</v>
+      </c>
+      <c r="E220">
+        <v>50000</v>
+      </c>
+      <c r="F220">
+        <v>20</v>
+      </c>
+      <c r="G220">
+        <v>15</v>
+      </c>
+      <c r="H220">
+        <v>20</v>
+      </c>
+      <c r="I220" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>16</v>
+      </c>
+      <c r="B221">
+        <v>474</v>
+      </c>
+      <c r="C221">
+        <v>370</v>
+      </c>
+      <c r="D221">
+        <v>49156</v>
+      </c>
+      <c r="E221">
+        <v>50000</v>
+      </c>
+      <c r="F221">
+        <v>20</v>
+      </c>
+      <c r="G221">
+        <v>15</v>
+      </c>
+      <c r="H221">
+        <v>20</v>
+      </c>
+      <c r="I221" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>17</v>
+      </c>
+      <c r="B222">
+        <v>471</v>
+      </c>
+      <c r="C222">
+        <v>388</v>
+      </c>
+      <c r="D222">
+        <v>49141</v>
+      </c>
+      <c r="E222">
+        <v>50000</v>
+      </c>
+      <c r="F222">
+        <v>20</v>
+      </c>
+      <c r="G222">
+        <v>15</v>
+      </c>
+      <c r="H222">
+        <v>20</v>
+      </c>
+      <c r="I222" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>18</v>
+      </c>
+      <c r="B223">
+        <v>413</v>
+      </c>
+      <c r="C223">
+        <v>384</v>
+      </c>
+      <c r="D223">
+        <v>49203</v>
+      </c>
+      <c r="E223">
+        <v>50000</v>
+      </c>
+      <c r="F223">
+        <v>20</v>
+      </c>
+      <c r="G223">
+        <v>15</v>
+      </c>
+      <c r="H223">
+        <v>20</v>
+      </c>
+      <c r="I223" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>19</v>
+      </c>
+      <c r="B224">
+        <v>447</v>
+      </c>
+      <c r="C224">
+        <v>366</v>
+      </c>
+      <c r="D224">
+        <v>49187</v>
+      </c>
+      <c r="E224">
+        <v>50000</v>
+      </c>
+      <c r="F224">
+        <v>20</v>
+      </c>
+      <c r="G224">
+        <v>15</v>
+      </c>
+      <c r="H224">
+        <v>20</v>
+      </c>
+      <c r="I224" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>20</v>
+      </c>
+      <c r="B225">
+        <v>448</v>
+      </c>
+      <c r="C225">
+        <v>385</v>
+      </c>
+      <c r="D225">
+        <v>49167</v>
+      </c>
+      <c r="E225">
+        <v>50000</v>
+      </c>
+      <c r="F225">
+        <v>20</v>
+      </c>
+      <c r="G225">
+        <v>15</v>
+      </c>
+      <c r="H225">
+        <v>20</v>
+      </c>
+      <c r="I225" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>21</v>
+      </c>
+      <c r="B226">
+        <v>475</v>
+      </c>
+      <c r="C226">
+        <v>371</v>
+      </c>
+      <c r="D226">
+        <v>49154</v>
+      </c>
+      <c r="E226">
+        <v>50000</v>
+      </c>
+      <c r="F226">
+        <v>20</v>
+      </c>
+      <c r="G226">
+        <v>15</v>
+      </c>
+      <c r="H226">
+        <v>20</v>
+      </c>
+      <c r="I226" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>22</v>
+      </c>
+      <c r="B227">
+        <v>522</v>
+      </c>
+      <c r="C227">
+        <v>398</v>
+      </c>
+      <c r="D227">
+        <v>49080</v>
+      </c>
+      <c r="E227">
+        <v>50000</v>
+      </c>
+      <c r="F227">
+        <v>20</v>
+      </c>
+      <c r="G227">
+        <v>15</v>
+      </c>
+      <c r="H227">
+        <v>20</v>
+      </c>
+      <c r="I227" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>23</v>
+      </c>
+      <c r="B228">
+        <v>466</v>
+      </c>
+      <c r="C228">
+        <v>381</v>
+      </c>
+      <c r="D228">
+        <v>49153</v>
+      </c>
+      <c r="E228">
+        <v>50000</v>
+      </c>
+      <c r="F228">
+        <v>20</v>
+      </c>
+      <c r="G228">
+        <v>15</v>
+      </c>
+      <c r="H228">
+        <v>20</v>
+      </c>
+      <c r="I228" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>24</v>
+      </c>
+      <c r="B229">
+        <v>475</v>
+      </c>
+      <c r="C229">
+        <v>355</v>
+      </c>
+      <c r="D229">
+        <v>49170</v>
+      </c>
+      <c r="E229">
+        <v>50000</v>
+      </c>
+      <c r="F229">
+        <v>20</v>
+      </c>
+      <c r="G229">
+        <v>15</v>
+      </c>
+      <c r="H229">
+        <v>20</v>
+      </c>
+      <c r="I229" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>25</v>
+      </c>
+      <c r="B230">
+        <v>414</v>
+      </c>
+      <c r="C230">
+        <v>392</v>
+      </c>
+      <c r="D230">
+        <v>49194</v>
+      </c>
+      <c r="E230">
+        <v>50000</v>
+      </c>
+      <c r="F230">
+        <v>20</v>
+      </c>
+      <c r="G230">
+        <v>15</v>
+      </c>
+      <c r="H230">
+        <v>20</v>
+      </c>
+      <c r="I230" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>26</v>
+      </c>
+      <c r="B231">
+        <v>480</v>
+      </c>
+      <c r="C231">
+        <v>368</v>
+      </c>
+      <c r="D231">
+        <v>49152</v>
+      </c>
+      <c r="E231">
+        <v>50000</v>
+      </c>
+      <c r="F231">
+        <v>20</v>
+      </c>
+      <c r="G231">
+        <v>15</v>
+      </c>
+      <c r="H231">
+        <v>20</v>
+      </c>
+      <c r="I231" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>27</v>
+      </c>
+      <c r="B232">
+        <v>458</v>
+      </c>
+      <c r="C232">
+        <v>428</v>
+      </c>
+      <c r="D232">
+        <v>49114</v>
+      </c>
+      <c r="E232">
+        <v>50000</v>
+      </c>
+      <c r="F232">
+        <v>20</v>
+      </c>
+      <c r="G232">
+        <v>15</v>
+      </c>
+      <c r="H232">
+        <v>20</v>
+      </c>
+      <c r="I232" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>28</v>
+      </c>
+      <c r="B233">
+        <v>489</v>
+      </c>
+      <c r="C233">
+        <v>384</v>
+      </c>
+      <c r="D233">
+        <v>49127</v>
+      </c>
+      <c r="E233">
+        <v>50000</v>
+      </c>
+      <c r="F233">
+        <v>20</v>
+      </c>
+      <c r="G233">
+        <v>15</v>
+      </c>
+      <c r="H233">
+        <v>20</v>
+      </c>
+      <c r="I233" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>29</v>
+      </c>
+      <c r="B234">
+        <v>491</v>
+      </c>
+      <c r="C234">
+        <v>367</v>
+      </c>
+      <c r="D234">
+        <v>49142</v>
+      </c>
+      <c r="E234">
+        <v>50000</v>
+      </c>
+      <c r="F234">
+        <v>20</v>
+      </c>
+      <c r="G234">
+        <v>15</v>
+      </c>
+      <c r="H234">
+        <v>20</v>
+      </c>
+      <c r="I234" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>30</v>
+      </c>
+      <c r="B235">
+        <v>481</v>
+      </c>
+      <c r="C235">
+        <v>366</v>
+      </c>
+      <c r="D235">
+        <v>49153</v>
+      </c>
+      <c r="E235">
+        <v>50000</v>
+      </c>
+      <c r="F235">
+        <v>20</v>
+      </c>
+      <c r="G235">
+        <v>15</v>
+      </c>
+      <c r="H235">
+        <v>20</v>
+      </c>
+      <c r="I235" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>31</v>
+      </c>
+      <c r="B236">
+        <v>441</v>
+      </c>
+      <c r="C236">
+        <v>392</v>
+      </c>
+      <c r="D236">
+        <v>49167</v>
+      </c>
+      <c r="E236">
+        <v>50000</v>
+      </c>
+      <c r="F236">
+        <v>20</v>
+      </c>
+      <c r="G236">
+        <v>15</v>
+      </c>
+      <c r="H236">
+        <v>20</v>
+      </c>
+      <c r="I236" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>32</v>
+      </c>
+      <c r="B237">
+        <v>499</v>
+      </c>
+      <c r="C237">
+        <v>406</v>
+      </c>
+      <c r="D237">
+        <v>49095</v>
+      </c>
+      <c r="E237">
+        <v>50000</v>
+      </c>
+      <c r="F237">
+        <v>20</v>
+      </c>
+      <c r="G237">
+        <v>15</v>
+      </c>
+      <c r="H237">
+        <v>20</v>
+      </c>
+      <c r="I237" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>33</v>
+      </c>
+      <c r="B238">
+        <v>450</v>
+      </c>
+      <c r="C238">
+        <v>406</v>
+      </c>
+      <c r="D238">
+        <v>49144</v>
+      </c>
+      <c r="E238">
+        <v>50000</v>
+      </c>
+      <c r="F238">
+        <v>20</v>
+      </c>
+      <c r="G238">
+        <v>15</v>
+      </c>
+      <c r="H238">
+        <v>20</v>
+      </c>
+      <c r="I238" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>34</v>
+      </c>
+      <c r="B239">
+        <v>455</v>
+      </c>
+      <c r="C239">
+        <v>372</v>
+      </c>
+      <c r="D239">
+        <v>49173</v>
+      </c>
+      <c r="E239">
+        <v>50000</v>
+      </c>
+      <c r="F239">
+        <v>20</v>
+      </c>
+      <c r="G239">
+        <v>15</v>
+      </c>
+      <c r="H239">
+        <v>20</v>
+      </c>
+      <c r="I239" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>35</v>
+      </c>
+      <c r="B240">
+        <v>466</v>
+      </c>
+      <c r="C240">
+        <v>414</v>
+      </c>
+      <c r="D240">
+        <v>49120</v>
+      </c>
+      <c r="E240">
+        <v>50000</v>
+      </c>
+      <c r="F240">
+        <v>20</v>
+      </c>
+      <c r="G240">
+        <v>15</v>
+      </c>
+      <c r="H240">
+        <v>20</v>
+      </c>
+      <c r="I240" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>36</v>
+      </c>
+      <c r="B241">
+        <v>478</v>
+      </c>
+      <c r="C241">
+        <v>429</v>
+      </c>
+      <c r="D241">
+        <v>49093</v>
+      </c>
+      <c r="E241">
+        <v>50000</v>
+      </c>
+      <c r="F241">
+        <v>20</v>
+      </c>
+      <c r="G241">
+        <v>15</v>
+      </c>
+      <c r="H241">
+        <v>20</v>
+      </c>
+      <c r="I241" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>37</v>
+      </c>
+      <c r="B242">
+        <v>456</v>
+      </c>
+      <c r="C242">
+        <v>407</v>
+      </c>
+      <c r="D242">
+        <v>49137</v>
+      </c>
+      <c r="E242">
+        <v>50000</v>
+      </c>
+      <c r="F242">
+        <v>20</v>
+      </c>
+      <c r="G242">
+        <v>15</v>
+      </c>
+      <c r="H242">
+        <v>20</v>
+      </c>
+      <c r="I242" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>38</v>
+      </c>
+      <c r="B243">
+        <v>490</v>
+      </c>
+      <c r="C243">
+        <v>391</v>
+      </c>
+      <c r="D243">
+        <v>49119</v>
+      </c>
+      <c r="E243">
+        <v>50000</v>
+      </c>
+      <c r="F243">
+        <v>20</v>
+      </c>
+      <c r="G243">
+        <v>15</v>
+      </c>
+      <c r="H243">
+        <v>20</v>
+      </c>
+      <c r="I243" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>39</v>
+      </c>
+      <c r="B244">
+        <v>471</v>
+      </c>
+      <c r="C244">
+        <v>404</v>
+      </c>
+      <c r="D244">
+        <v>49125</v>
+      </c>
+      <c r="E244">
+        <v>50000</v>
+      </c>
+      <c r="F244">
+        <v>20</v>
+      </c>
+      <c r="G244">
+        <v>15</v>
+      </c>
+      <c r="H244">
+        <v>20</v>
+      </c>
+      <c r="I244" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>40</v>
+      </c>
+      <c r="B245">
+        <v>451</v>
+      </c>
+      <c r="C245">
+        <v>379</v>
+      </c>
+      <c r="D245">
+        <v>49170</v>
+      </c>
+      <c r="E245">
+        <v>50000</v>
+      </c>
+      <c r="F245">
+        <v>20</v>
+      </c>
+      <c r="G245">
+        <v>15</v>
+      </c>
+      <c r="H245">
+        <v>20</v>
+      </c>
+      <c r="I245" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>41</v>
+      </c>
+      <c r="B246">
+        <v>470</v>
+      </c>
+      <c r="C246">
+        <v>362</v>
+      </c>
+      <c r="D246">
+        <v>49168</v>
+      </c>
+      <c r="E246">
+        <v>50000</v>
+      </c>
+      <c r="F246">
+        <v>20</v>
+      </c>
+      <c r="G246">
+        <v>15</v>
+      </c>
+      <c r="H246">
+        <v>20</v>
+      </c>
+      <c r="I246" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>42</v>
+      </c>
+      <c r="B247">
+        <v>463</v>
+      </c>
+      <c r="C247">
+        <v>427</v>
+      </c>
+      <c r="D247">
+        <v>49110</v>
+      </c>
+      <c r="E247">
+        <v>50000</v>
+      </c>
+      <c r="F247">
+        <v>20</v>
+      </c>
+      <c r="G247">
+        <v>15</v>
+      </c>
+      <c r="H247">
+        <v>20</v>
+      </c>
+      <c r="I247" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>43</v>
+      </c>
+      <c r="B248">
+        <v>457</v>
+      </c>
+      <c r="C248">
+        <v>390</v>
+      </c>
+      <c r="D248">
+        <v>49153</v>
+      </c>
+      <c r="E248">
+        <v>50000</v>
+      </c>
+      <c r="F248">
+        <v>20</v>
+      </c>
+      <c r="G248">
+        <v>15</v>
+      </c>
+      <c r="H248">
+        <v>20</v>
+      </c>
+      <c r="I248" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>44</v>
+      </c>
+      <c r="B249">
+        <v>467</v>
+      </c>
+      <c r="C249">
+        <v>370</v>
+      </c>
+      <c r="D249">
+        <v>49163</v>
+      </c>
+      <c r="E249">
+        <v>50000</v>
+      </c>
+      <c r="F249">
+        <v>20</v>
+      </c>
+      <c r="G249">
+        <v>15</v>
+      </c>
+      <c r="H249">
+        <v>20</v>
+      </c>
+      <c r="I249" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>45</v>
+      </c>
+      <c r="B250">
+        <v>457</v>
+      </c>
+      <c r="C250">
+        <v>395</v>
+      </c>
+      <c r="D250">
+        <v>49148</v>
+      </c>
+      <c r="E250">
+        <v>50000</v>
+      </c>
+      <c r="F250">
+        <v>20</v>
+      </c>
+      <c r="G250">
+        <v>15</v>
+      </c>
+      <c r="H250">
+        <v>20</v>
+      </c>
+      <c r="I250" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>46</v>
+      </c>
+      <c r="B251">
+        <v>508</v>
+      </c>
+      <c r="C251">
+        <v>395</v>
+      </c>
+      <c r="D251">
+        <v>49097</v>
+      </c>
+      <c r="E251">
+        <v>50000</v>
+      </c>
+      <c r="F251">
+        <v>20</v>
+      </c>
+      <c r="G251">
+        <v>15</v>
+      </c>
+      <c r="H251">
+        <v>20</v>
+      </c>
+      <c r="I251" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>47</v>
+      </c>
+      <c r="B252">
+        <v>465</v>
+      </c>
+      <c r="C252">
+        <v>344</v>
+      </c>
+      <c r="D252">
+        <v>49191</v>
+      </c>
+      <c r="E252">
+        <v>50000</v>
+      </c>
+      <c r="F252">
+        <v>20</v>
+      </c>
+      <c r="G252">
+        <v>15</v>
+      </c>
+      <c r="H252">
+        <v>20</v>
+      </c>
+      <c r="I252" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>48</v>
+      </c>
+      <c r="B253">
+        <v>485</v>
+      </c>
+      <c r="C253">
+        <v>348</v>
+      </c>
+      <c r="D253">
+        <v>49167</v>
+      </c>
+      <c r="E253">
+        <v>50000</v>
+      </c>
+      <c r="F253">
+        <v>20</v>
+      </c>
+      <c r="G253">
+        <v>15</v>
+      </c>
+      <c r="H253">
+        <v>20</v>
+      </c>
+      <c r="I253" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>49</v>
+      </c>
+      <c r="B254">
+        <v>474</v>
+      </c>
+      <c r="C254">
+        <v>377</v>
+      </c>
+      <c r="D254">
+        <v>49149</v>
+      </c>
+      <c r="E254">
+        <v>50000</v>
+      </c>
+      <c r="F254">
+        <v>20</v>
+      </c>
+      <c r="G254">
+        <v>15</v>
+      </c>
+      <c r="H254">
+        <v>20</v>
+      </c>
+      <c r="I254" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>50</v>
+      </c>
+      <c r="B255">
+        <v>479</v>
+      </c>
+      <c r="C255">
+        <v>366</v>
+      </c>
+      <c r="D255">
+        <v>49155</v>
+      </c>
+      <c r="E255">
+        <v>50000</v>
+      </c>
+      <c r="F255">
+        <v>20</v>
+      </c>
+      <c r="G255">
+        <v>15</v>
+      </c>
+      <c r="H255">
+        <v>20</v>
+      </c>
+      <c r="I255" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>1</v>
+      </c>
+      <c r="B257">
+        <v>3880</v>
+      </c>
+      <c r="C257">
+        <v>3934</v>
+      </c>
+      <c r="D257">
+        <v>42186</v>
+      </c>
+      <c r="E257">
+        <v>50000</v>
+      </c>
+      <c r="F257">
+        <v>20</v>
+      </c>
+      <c r="G257">
+        <v>15</v>
+      </c>
+      <c r="H257">
+        <v>20</v>
+      </c>
+      <c r="I257" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>2</v>
+      </c>
+      <c r="B258">
+        <v>3899</v>
+      </c>
+      <c r="C258">
+        <v>3888</v>
+      </c>
+      <c r="D258">
+        <v>42213</v>
+      </c>
+      <c r="E258">
+        <v>50000</v>
+      </c>
+      <c r="F258">
+        <v>20</v>
+      </c>
+      <c r="G258">
+        <v>15</v>
+      </c>
+      <c r="H258">
+        <v>20</v>
+      </c>
+      <c r="I258" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>3</v>
+      </c>
+      <c r="B259">
+        <v>3958</v>
+      </c>
+      <c r="C259">
+        <v>3807</v>
+      </c>
+      <c r="D259">
+        <v>42235</v>
+      </c>
+      <c r="E259">
+        <v>50000</v>
+      </c>
+      <c r="F259">
+        <v>20</v>
+      </c>
+      <c r="G259">
+        <v>15</v>
+      </c>
+      <c r="H259">
+        <v>20</v>
+      </c>
+      <c r="I259" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>4</v>
+      </c>
+      <c r="B260">
+        <v>3886</v>
+      </c>
+      <c r="C260">
+        <v>3769</v>
+      </c>
+      <c r="D260">
+        <v>42345</v>
+      </c>
+      <c r="E260">
+        <v>50000</v>
+      </c>
+      <c r="F260">
+        <v>20</v>
+      </c>
+      <c r="G260">
+        <v>15</v>
+      </c>
+      <c r="H260">
+        <v>20</v>
+      </c>
+      <c r="I260" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>5</v>
+      </c>
+      <c r="B261">
+        <v>3933</v>
+      </c>
+      <c r="C261">
+        <v>3897</v>
+      </c>
+      <c r="D261">
+        <v>42170</v>
+      </c>
+      <c r="E261">
+        <v>50000</v>
+      </c>
+      <c r="F261">
+        <v>20</v>
+      </c>
+      <c r="G261">
+        <v>15</v>
+      </c>
+      <c r="H261">
+        <v>20</v>
+      </c>
+      <c r="I261" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>6</v>
+      </c>
+      <c r="B262">
+        <v>3874</v>
+      </c>
+      <c r="C262">
+        <v>3914</v>
+      </c>
+      <c r="D262">
+        <v>42212</v>
+      </c>
+      <c r="E262">
+        <v>50000</v>
+      </c>
+      <c r="F262">
+        <v>20</v>
+      </c>
+      <c r="G262">
+        <v>15</v>
+      </c>
+      <c r="H262">
+        <v>20</v>
+      </c>
+      <c r="I262" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>7</v>
+      </c>
+      <c r="B263">
+        <v>3896</v>
+      </c>
+      <c r="C263">
+        <v>3965</v>
+      </c>
+      <c r="D263">
+        <v>42139</v>
+      </c>
+      <c r="E263">
+        <v>50000</v>
+      </c>
+      <c r="F263">
+        <v>20</v>
+      </c>
+      <c r="G263">
+        <v>15</v>
+      </c>
+      <c r="H263">
+        <v>20</v>
+      </c>
+      <c r="I263" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>8</v>
+      </c>
+      <c r="B264">
+        <v>3937</v>
+      </c>
+      <c r="C264">
+        <v>3900</v>
+      </c>
+      <c r="D264">
+        <v>42163</v>
+      </c>
+      <c r="E264">
+        <v>50000</v>
+      </c>
+      <c r="F264">
+        <v>20</v>
+      </c>
+      <c r="G264">
+        <v>15</v>
+      </c>
+      <c r="H264">
+        <v>20</v>
+      </c>
+      <c r="I264" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>9</v>
+      </c>
+      <c r="B265">
+        <v>3880</v>
+      </c>
+      <c r="C265">
+        <v>3778</v>
+      </c>
+      <c r="D265">
+        <v>42342</v>
+      </c>
+      <c r="E265">
+        <v>50000</v>
+      </c>
+      <c r="F265">
+        <v>20</v>
+      </c>
+      <c r="G265">
+        <v>15</v>
+      </c>
+      <c r="H265">
+        <v>20</v>
+      </c>
+      <c r="I265" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>10</v>
+      </c>
+      <c r="B266">
+        <v>3938</v>
+      </c>
+      <c r="C266">
+        <v>3935</v>
+      </c>
+      <c r="D266">
+        <v>42127</v>
+      </c>
+      <c r="E266">
+        <v>50000</v>
+      </c>
+      <c r="F266">
+        <v>20</v>
+      </c>
+      <c r="G266">
+        <v>15</v>
+      </c>
+      <c r="H266">
+        <v>20</v>
+      </c>
+      <c r="I266" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>11</v>
+      </c>
+      <c r="B267">
+        <v>3947</v>
+      </c>
+      <c r="C267">
+        <v>3899</v>
+      </c>
+      <c r="D267">
+        <v>42154</v>
+      </c>
+      <c r="E267">
+        <v>50000</v>
+      </c>
+      <c r="F267">
+        <v>20</v>
+      </c>
+      <c r="G267">
+        <v>15</v>
+      </c>
+      <c r="H267">
+        <v>20</v>
+      </c>
+      <c r="I267" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>12</v>
+      </c>
+      <c r="B268">
+        <v>3939</v>
+      </c>
+      <c r="C268">
+        <v>3867</v>
+      </c>
+      <c r="D268">
+        <v>42194</v>
+      </c>
+      <c r="E268">
+        <v>50000</v>
+      </c>
+      <c r="F268">
+        <v>20</v>
+      </c>
+      <c r="G268">
+        <v>15</v>
+      </c>
+      <c r="H268">
+        <v>20</v>
+      </c>
+      <c r="I268" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>13</v>
+      </c>
+      <c r="B269">
+        <v>3940</v>
+      </c>
+      <c r="C269">
+        <v>3880</v>
+      </c>
+      <c r="D269">
+        <v>42180</v>
+      </c>
+      <c r="E269">
+        <v>50000</v>
+      </c>
+      <c r="F269">
+        <v>20</v>
+      </c>
+      <c r="G269">
+        <v>15</v>
+      </c>
+      <c r="H269">
+        <v>20</v>
+      </c>
+      <c r="I269" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>14</v>
+      </c>
+      <c r="B270">
+        <v>3907</v>
+      </c>
+      <c r="C270">
+        <v>3793</v>
+      </c>
+      <c r="D270">
+        <v>42300</v>
+      </c>
+      <c r="E270">
+        <v>50000</v>
+      </c>
+      <c r="F270">
+        <v>20</v>
+      </c>
+      <c r="G270">
+        <v>15</v>
+      </c>
+      <c r="H270">
+        <v>20</v>
+      </c>
+      <c r="I270" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>15</v>
+      </c>
+      <c r="B271">
+        <v>3815</v>
+      </c>
+      <c r="C271">
+        <v>3893</v>
+      </c>
+      <c r="D271">
+        <v>42292</v>
+      </c>
+      <c r="E271">
+        <v>50000</v>
+      </c>
+      <c r="F271">
+        <v>20</v>
+      </c>
+      <c r="G271">
+        <v>15</v>
+      </c>
+      <c r="H271">
+        <v>20</v>
+      </c>
+      <c r="I271" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>16</v>
+      </c>
+      <c r="B272">
+        <v>3951</v>
+      </c>
+      <c r="C272">
+        <v>3843</v>
+      </c>
+      <c r="D272">
+        <v>42206</v>
+      </c>
+      <c r="E272">
+        <v>50000</v>
+      </c>
+      <c r="F272">
+        <v>20</v>
+      </c>
+      <c r="G272">
+        <v>15</v>
+      </c>
+      <c r="H272">
+        <v>20</v>
+      </c>
+      <c r="I272" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>17</v>
+      </c>
+      <c r="B273">
+        <v>3867</v>
+      </c>
+      <c r="C273">
+        <v>3913</v>
+      </c>
+      <c r="D273">
+        <v>42220</v>
+      </c>
+      <c r="E273">
+        <v>50000</v>
+      </c>
+      <c r="F273">
+        <v>20</v>
+      </c>
+      <c r="G273">
+        <v>15</v>
+      </c>
+      <c r="H273">
+        <v>20</v>
+      </c>
+      <c r="I273" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>18</v>
+      </c>
+      <c r="B274">
+        <v>3886</v>
+      </c>
+      <c r="C274">
+        <v>3938</v>
+      </c>
+      <c r="D274">
+        <v>42176</v>
+      </c>
+      <c r="E274">
+        <v>50000</v>
+      </c>
+      <c r="F274">
+        <v>20</v>
+      </c>
+      <c r="G274">
+        <v>15</v>
+      </c>
+      <c r="H274">
+        <v>20</v>
+      </c>
+      <c r="I274" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>19</v>
+      </c>
+      <c r="B275">
+        <v>3916</v>
+      </c>
+      <c r="C275">
+        <v>3895</v>
+      </c>
+      <c r="D275">
+        <v>42189</v>
+      </c>
+      <c r="E275">
+        <v>50000</v>
+      </c>
+      <c r="F275">
+        <v>20</v>
+      </c>
+      <c r="G275">
+        <v>15</v>
+      </c>
+      <c r="H275">
+        <v>20</v>
+      </c>
+      <c r="I275" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>20</v>
+      </c>
+      <c r="B276">
+        <v>3948</v>
+      </c>
+      <c r="C276">
+        <v>3895</v>
+      </c>
+      <c r="D276">
+        <v>42157</v>
+      </c>
+      <c r="E276">
+        <v>50000</v>
+      </c>
+      <c r="F276">
+        <v>20</v>
+      </c>
+      <c r="G276">
+        <v>15</v>
+      </c>
+      <c r="H276">
+        <v>20</v>
+      </c>
+      <c r="I276" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>21</v>
+      </c>
+      <c r="B277">
+        <v>3820</v>
+      </c>
+      <c r="C277">
+        <v>3809</v>
+      </c>
+      <c r="D277">
+        <v>42371</v>
+      </c>
+      <c r="E277">
+        <v>50000</v>
+      </c>
+      <c r="F277">
+        <v>20</v>
+      </c>
+      <c r="G277">
+        <v>15</v>
+      </c>
+      <c r="H277">
+        <v>20</v>
+      </c>
+      <c r="I277" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>22</v>
+      </c>
+      <c r="B278">
+        <v>3966</v>
+      </c>
+      <c r="C278">
+        <v>3855</v>
+      </c>
+      <c r="D278">
+        <v>42179</v>
+      </c>
+      <c r="E278">
+        <v>50000</v>
+      </c>
+      <c r="F278">
+        <v>20</v>
+      </c>
+      <c r="G278">
+        <v>15</v>
+      </c>
+      <c r="H278">
+        <v>20</v>
+      </c>
+      <c r="I278" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>23</v>
+      </c>
+      <c r="B279">
+        <v>4016</v>
+      </c>
+      <c r="C279">
+        <v>3904</v>
+      </c>
+      <c r="D279">
+        <v>42080</v>
+      </c>
+      <c r="E279">
+        <v>50000</v>
+      </c>
+      <c r="F279">
+        <v>20</v>
+      </c>
+      <c r="G279">
+        <v>15</v>
+      </c>
+      <c r="H279">
+        <v>20</v>
+      </c>
+      <c r="I279" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>24</v>
+      </c>
+      <c r="B280">
+        <v>3788</v>
+      </c>
+      <c r="C280">
+        <v>3998</v>
+      </c>
+      <c r="D280">
+        <v>42214</v>
+      </c>
+      <c r="E280">
+        <v>50000</v>
+      </c>
+      <c r="F280">
+        <v>20</v>
+      </c>
+      <c r="G280">
+        <v>15</v>
+      </c>
+      <c r="H280">
+        <v>20</v>
+      </c>
+      <c r="I280" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>25</v>
+      </c>
+      <c r="B281">
+        <v>3914</v>
+      </c>
+      <c r="C281">
+        <v>3781</v>
+      </c>
+      <c r="D281">
+        <v>42305</v>
+      </c>
+      <c r="E281">
+        <v>50000</v>
+      </c>
+      <c r="F281">
+        <v>20</v>
+      </c>
+      <c r="G281">
+        <v>15</v>
+      </c>
+      <c r="H281">
+        <v>20</v>
+      </c>
+      <c r="I281" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>26</v>
+      </c>
+      <c r="B282">
+        <v>3926</v>
+      </c>
+      <c r="C282">
+        <v>3788</v>
+      </c>
+      <c r="D282">
+        <v>42286</v>
+      </c>
+      <c r="E282">
+        <v>50000</v>
+      </c>
+      <c r="F282">
+        <v>20</v>
+      </c>
+      <c r="G282">
+        <v>15</v>
+      </c>
+      <c r="H282">
+        <v>20</v>
+      </c>
+      <c r="I282" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>27</v>
+      </c>
+      <c r="B283">
+        <v>3938</v>
+      </c>
+      <c r="C283">
+        <v>3857</v>
+      </c>
+      <c r="D283">
+        <v>42205</v>
+      </c>
+      <c r="E283">
+        <v>50000</v>
+      </c>
+      <c r="F283">
+        <v>20</v>
+      </c>
+      <c r="G283">
+        <v>15</v>
+      </c>
+      <c r="H283">
+        <v>20</v>
+      </c>
+      <c r="I283" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>28</v>
+      </c>
+      <c r="B284">
+        <v>3864</v>
+      </c>
+      <c r="C284">
+        <v>3964</v>
+      </c>
+      <c r="D284">
+        <v>42172</v>
+      </c>
+      <c r="E284">
+        <v>50000</v>
+      </c>
+      <c r="F284">
+        <v>20</v>
+      </c>
+      <c r="G284">
+        <v>15</v>
+      </c>
+      <c r="H284">
+        <v>20</v>
+      </c>
+      <c r="I284" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>29</v>
+      </c>
+      <c r="B285">
+        <v>3964</v>
+      </c>
+      <c r="C285">
+        <v>3878</v>
+      </c>
+      <c r="D285">
+        <v>42158</v>
+      </c>
+      <c r="E285">
+        <v>50000</v>
+      </c>
+      <c r="F285">
+        <v>20</v>
+      </c>
+      <c r="G285">
+        <v>15</v>
+      </c>
+      <c r="H285">
+        <v>20</v>
+      </c>
+      <c r="I285" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>30</v>
+      </c>
+      <c r="B286">
+        <v>3842</v>
+      </c>
+      <c r="C286">
+        <v>3871</v>
+      </c>
+      <c r="D286">
+        <v>42287</v>
+      </c>
+      <c r="E286">
+        <v>50000</v>
+      </c>
+      <c r="F286">
+        <v>20</v>
+      </c>
+      <c r="G286">
+        <v>15</v>
+      </c>
+      <c r="H286">
+        <v>20</v>
+      </c>
+      <c r="I286" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>31</v>
+      </c>
+      <c r="B287">
+        <v>3986</v>
+      </c>
+      <c r="C287">
+        <v>3879</v>
+      </c>
+      <c r="D287">
+        <v>42135</v>
+      </c>
+      <c r="E287">
+        <v>50000</v>
+      </c>
+      <c r="F287">
+        <v>20</v>
+      </c>
+      <c r="G287">
+        <v>15</v>
+      </c>
+      <c r="H287">
+        <v>20</v>
+      </c>
+      <c r="I287" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>32</v>
+      </c>
+      <c r="B288">
+        <v>3904</v>
+      </c>
+      <c r="C288">
+        <v>4006</v>
+      </c>
+      <c r="D288">
+        <v>42090</v>
+      </c>
+      <c r="E288">
+        <v>50000</v>
+      </c>
+      <c r="F288">
+        <v>20</v>
+      </c>
+      <c r="G288">
+        <v>15</v>
+      </c>
+      <c r="H288">
+        <v>20</v>
+      </c>
+      <c r="I288" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>33</v>
+      </c>
+      <c r="B289">
+        <v>3846</v>
+      </c>
+      <c r="C289">
+        <v>3958</v>
+      </c>
+      <c r="D289">
+        <v>42196</v>
+      </c>
+      <c r="E289">
+        <v>50000</v>
+      </c>
+      <c r="F289">
+        <v>20</v>
+      </c>
+      <c r="G289">
+        <v>15</v>
+      </c>
+      <c r="H289">
+        <v>20</v>
+      </c>
+      <c r="I289" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>34</v>
+      </c>
+      <c r="B290">
+        <v>3953</v>
+      </c>
+      <c r="C290">
+        <v>3849</v>
+      </c>
+      <c r="D290">
+        <v>42198</v>
+      </c>
+      <c r="E290">
+        <v>50000</v>
+      </c>
+      <c r="F290">
+        <v>20</v>
+      </c>
+      <c r="G290">
+        <v>15</v>
+      </c>
+      <c r="H290">
+        <v>20</v>
+      </c>
+      <c r="I290" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>35</v>
+      </c>
+      <c r="B291">
+        <v>3813</v>
+      </c>
+      <c r="C291">
+        <v>3978</v>
+      </c>
+      <c r="D291">
+        <v>42209</v>
+      </c>
+      <c r="E291">
+        <v>50000</v>
+      </c>
+      <c r="F291">
+        <v>20</v>
+      </c>
+      <c r="G291">
+        <v>15</v>
+      </c>
+      <c r="H291">
+        <v>20</v>
+      </c>
+      <c r="I291" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>36</v>
+      </c>
+      <c r="B292">
+        <v>3945</v>
+      </c>
+      <c r="C292">
+        <v>3991</v>
+      </c>
+      <c r="D292">
+        <v>42064</v>
+      </c>
+      <c r="E292">
+        <v>50000</v>
+      </c>
+      <c r="F292">
+        <v>20</v>
+      </c>
+      <c r="G292">
+        <v>15</v>
+      </c>
+      <c r="H292">
+        <v>20</v>
+      </c>
+      <c r="I292" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>37</v>
+      </c>
+      <c r="B293">
+        <v>3925</v>
+      </c>
+      <c r="C293">
+        <v>3799</v>
+      </c>
+      <c r="D293">
+        <v>42276</v>
+      </c>
+      <c r="E293">
+        <v>50000</v>
+      </c>
+      <c r="F293">
+        <v>20</v>
+      </c>
+      <c r="G293">
+        <v>15</v>
+      </c>
+      <c r="H293">
+        <v>20</v>
+      </c>
+      <c r="I293" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>38</v>
+      </c>
+      <c r="B294">
+        <v>3911</v>
+      </c>
+      <c r="C294">
+        <v>3944</v>
+      </c>
+      <c r="D294">
+        <v>42145</v>
+      </c>
+      <c r="E294">
+        <v>50000</v>
+      </c>
+      <c r="F294">
+        <v>20</v>
+      </c>
+      <c r="G294">
+        <v>15</v>
+      </c>
+      <c r="H294">
+        <v>20</v>
+      </c>
+      <c r="I294" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>39</v>
+      </c>
+      <c r="B295">
+        <v>3857</v>
+      </c>
+      <c r="C295">
+        <v>3761</v>
+      </c>
+      <c r="D295">
+        <v>42382</v>
+      </c>
+      <c r="E295">
+        <v>50000</v>
+      </c>
+      <c r="F295">
+        <v>20</v>
+      </c>
+      <c r="G295">
+        <v>15</v>
+      </c>
+      <c r="H295">
+        <v>20</v>
+      </c>
+      <c r="I295" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>40</v>
+      </c>
+      <c r="B296">
+        <v>3946</v>
+      </c>
+      <c r="C296">
+        <v>3839</v>
+      </c>
+      <c r="D296">
+        <v>42215</v>
+      </c>
+      <c r="E296">
+        <v>50000</v>
+      </c>
+      <c r="F296">
+        <v>20</v>
+      </c>
+      <c r="G296">
+        <v>15</v>
+      </c>
+      <c r="H296">
+        <v>20</v>
+      </c>
+      <c r="I296" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>41</v>
+      </c>
+      <c r="B297">
+        <v>3853</v>
+      </c>
+      <c r="C297">
+        <v>3824</v>
+      </c>
+      <c r="D297">
+        <v>42323</v>
+      </c>
+      <c r="E297">
+        <v>50000</v>
+      </c>
+      <c r="F297">
+        <v>20</v>
+      </c>
+      <c r="G297">
+        <v>15</v>
+      </c>
+      <c r="H297">
+        <v>20</v>
+      </c>
+      <c r="I297" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>42</v>
+      </c>
+      <c r="B298">
+        <v>3816</v>
+      </c>
+      <c r="C298">
+        <v>3877</v>
+      </c>
+      <c r="D298">
+        <v>42307</v>
+      </c>
+      <c r="E298">
+        <v>50000</v>
+      </c>
+      <c r="F298">
+        <v>20</v>
+      </c>
+      <c r="G298">
+        <v>15</v>
+      </c>
+      <c r="H298">
+        <v>20</v>
+      </c>
+      <c r="I298" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>43</v>
+      </c>
+      <c r="B299">
+        <v>3903</v>
+      </c>
+      <c r="C299">
+        <v>3863</v>
+      </c>
+      <c r="D299">
+        <v>42234</v>
+      </c>
+      <c r="E299">
+        <v>50000</v>
+      </c>
+      <c r="F299">
+        <v>20</v>
+      </c>
+      <c r="G299">
+        <v>15</v>
+      </c>
+      <c r="H299">
+        <v>20</v>
+      </c>
+      <c r="I299" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>44</v>
+      </c>
+      <c r="B300">
+        <v>3865</v>
+      </c>
+      <c r="C300">
+        <v>3764</v>
+      </c>
+      <c r="D300">
+        <v>42371</v>
+      </c>
+      <c r="E300">
+        <v>50000</v>
+      </c>
+      <c r="F300">
+        <v>20</v>
+      </c>
+      <c r="G300">
+        <v>15</v>
+      </c>
+      <c r="H300">
+        <v>20</v>
+      </c>
+      <c r="I300" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>45</v>
+      </c>
+      <c r="B301">
+        <v>3961</v>
+      </c>
+      <c r="C301">
+        <v>3812</v>
+      </c>
+      <c r="D301">
+        <v>42227</v>
+      </c>
+      <c r="E301">
+        <v>50000</v>
+      </c>
+      <c r="F301">
+        <v>20</v>
+      </c>
+      <c r="G301">
+        <v>15</v>
+      </c>
+      <c r="H301">
+        <v>20</v>
+      </c>
+      <c r="I301" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>46</v>
+      </c>
+      <c r="B302">
+        <v>3955</v>
+      </c>
+      <c r="C302">
+        <v>3852</v>
+      </c>
+      <c r="D302">
+        <v>42193</v>
+      </c>
+      <c r="E302">
+        <v>50000</v>
+      </c>
+      <c r="F302">
+        <v>20</v>
+      </c>
+      <c r="G302">
+        <v>15</v>
+      </c>
+      <c r="H302">
+        <v>20</v>
+      </c>
+      <c r="I302" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>47</v>
+      </c>
+      <c r="B303">
+        <v>3880</v>
+      </c>
+      <c r="C303">
+        <v>3858</v>
+      </c>
+      <c r="D303">
+        <v>42262</v>
+      </c>
+      <c r="E303">
+        <v>50000</v>
+      </c>
+      <c r="F303">
+        <v>20</v>
+      </c>
+      <c r="G303">
+        <v>15</v>
+      </c>
+      <c r="H303">
+        <v>20</v>
+      </c>
+      <c r="I303" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>48</v>
+      </c>
+      <c r="B304">
+        <v>3905</v>
+      </c>
+      <c r="C304">
+        <v>3919</v>
+      </c>
+      <c r="D304">
+        <v>42176</v>
+      </c>
+      <c r="E304">
+        <v>50000</v>
+      </c>
+      <c r="F304">
+        <v>20</v>
+      </c>
+      <c r="G304">
+        <v>15</v>
+      </c>
+      <c r="H304">
+        <v>20</v>
+      </c>
+      <c r="I304" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>49</v>
+      </c>
+      <c r="B305">
+        <v>3870</v>
+      </c>
+      <c r="C305">
+        <v>3933</v>
+      </c>
+      <c r="D305">
+        <v>42197</v>
+      </c>
+      <c r="E305">
+        <v>50000</v>
+      </c>
+      <c r="F305">
+        <v>20</v>
+      </c>
+      <c r="G305">
+        <v>15</v>
+      </c>
+      <c r="H305">
+        <v>20</v>
+      </c>
+      <c r="I305" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>50</v>
+      </c>
+      <c r="B306">
+        <v>3826</v>
+      </c>
+      <c r="C306">
+        <v>3963</v>
+      </c>
+      <c r="D306">
+        <v>42211</v>
+      </c>
+      <c r="E306">
+        <v>50000</v>
+      </c>
+      <c r="F306">
+        <v>20</v>
+      </c>
+      <c r="G306">
+        <v>15</v>
+      </c>
+      <c r="H306">
+        <v>20</v>
+      </c>
+      <c r="I306" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>